<commit_message>
Addin some background info
</commit_message>
<xml_diff>
--- a/hv-psu-discrete/calc/maida-lm317/LT317-Maida.xlsx
+++ b/hv-psu-discrete/calc/maida-lm317/LT317-Maida.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schenk/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C681CD79-83EA-E141-B5D3-71C5AA669BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BFE481-D6A2-FD48-BC33-C685CE5F2971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{D14FE013-FA0C-1D41-8C6E-C9A2F15D763D}"/>
+    <workbookView xWindow="9920" yWindow="1280" windowWidth="28040" windowHeight="16080" xr2:uid="{CB4EBD37-40D9-F24E-B9F7-70AF855F51E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,21 +36,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>RV1</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>VOUT</t>
-  </si>
-  <si>
-    <t>PR4</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>Rvmin</t>
+  </si>
+  <si>
+    <t>Rvmax</t>
+  </si>
+  <si>
+    <t>VOUTmin</t>
+  </si>
+  <si>
+    <t>VOUTmax</t>
+  </si>
+  <si>
+    <t>PVR21</t>
+  </si>
+  <si>
+    <t>IR21</t>
+  </si>
+  <si>
+    <t>ILOADmin</t>
+  </si>
+  <si>
+    <t>LM317</t>
+  </si>
+  <si>
+    <t>10mA max to maintain regulation</t>
   </si>
 </sst>
 </file>
@@ -66,12 +84,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,8 +110,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,55 +428,365 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F5A1DD-8ACA-AF4C-817C-DE7EDAC7B665}">
-  <dimension ref="A4:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750EDE42-0368-7442-9A32-6C495C1CF73A}">
+  <dimension ref="A7:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>121</v>
+      </c>
+      <c r="B8" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>2000</v>
+      </c>
+      <c r="F8">
+        <f>1.25*(1+(C8+B8)/A8)</f>
+        <v>104.55578512396696</v>
+      </c>
+      <c r="G8">
+        <f>1.25*(1+(D8+B8)/A8)</f>
+        <v>125.21694214876034</v>
+      </c>
+      <c r="H8">
+        <f>(G8*G8)/B8</f>
+        <v>1.5679282601085993</v>
+      </c>
+      <c r="I8">
+        <f>G8/B8</f>
+        <v>1.2521694214876034E-2</v>
+      </c>
+      <c r="J8">
+        <f>G8/(B8+D8)</f>
+        <v>1.0434745179063362E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>121</v>
+      </c>
+      <c r="B9" s="1">
+        <v>12000</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>2000</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F34" si="0">1.25*(1+(C9+B9)/A9)</f>
+        <v>125.21694214876034</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9:G34" si="1">1.25*(1+(D9+B9)/A9)</f>
+        <v>145.87809917355372</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ref="H9:H34" si="2">(G9*G9)/B9</f>
+        <v>1.7733683182074313</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ref="I9:I34" si="3">G9/B9</f>
+        <v>1.2156508264462811E-2</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ref="J9:J34" si="4">G9/(B9+D9)</f>
+        <v>1.0419864226682408E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>121</v>
+      </c>
+      <c r="B10" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>2000</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>156.20867768595042</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>176.86983471074382</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>2.0855292287070557</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>1.1791322314049588E-2</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="4"/>
+        <v>1.0404107924161401E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>121</v>
+      </c>
+      <c r="B11" s="1">
         <v>18000</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <f>1.25*(1+(B4+B5)/B6)</f>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>2000</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>187.20041322314049</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
         <v>207.86157024793391</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <f>B7^2/B5</f>
+      <c r="H11">
+        <f t="shared" si="2"/>
         <v>2.4003573547742647</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>1.1547865013774106E-2</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="4"/>
+        <v>1.0393078512396696E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>121</v>
+      </c>
+      <c r="B12" s="1">
+        <v>22000</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>2000</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>228.52272727272725</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>249.18388429752068</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>2.8223912815272807</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>1.1326540195341848E-2</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="4"/>
+        <v>1.0382661845730029E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>121</v>
+      </c>
+      <c r="B13" s="1">
+        <v>27000</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>2000</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>280.17561983471074</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>300.83677685950414</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>3.3519543078227811</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>1.1142102846648301E-2</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="4"/>
+        <v>1.0373681960672556E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>121</v>
+      </c>
+      <c r="B14" s="1">
+        <v>33000</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>2000</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>342.15909090909093</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>362.82024793388427</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>3.9890464336607652</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>1.0994552967693463E-2</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="4"/>
+        <v>1.0366292798110979E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>121</v>
+      </c>
+      <c r="B15" s="1">
+        <v>39000</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>2000</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>404.14256198347107</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>424.80371900826447</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>4.6271333252116031</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>1.089240305149396E-2</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="4"/>
+        <v>1.0361066317274743E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>121</v>
+      </c>
+      <c r="B16" s="1">
+        <v>47000</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>2000</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>486.78719008264466</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>507.44834710743805</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>5.4788047868525735</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>1.0796773342711449E-2</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="4"/>
+        <v>1.0356088716478327E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>